<commit_message>
simulated observation code improved
</commit_message>
<xml_diff>
--- a/reports/SNR_measurement.xlsx
+++ b/reports/SNR_measurement.xlsx
@@ -67,10 +67,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
-    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -151,19 +150,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,217 +361,217 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="n">
+      <c r="B1" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="n">
+      <c r="C1" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>913</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <f aca="false">0.9*B2</f>
         <v>821.7</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>4.62</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>28.6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>604</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <f aca="false">0.9*B3</f>
         <v>543.6</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4.45</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>21.4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>444</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <f aca="false">0.9*B4</f>
         <v>399.6</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>3.66</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>17.87</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>639</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <f aca="false">0.9*B5</f>
         <v>575.1</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>4.41</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>22.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>605</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <f aca="false">0.9*B6</f>
         <v>544.5</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>2.52</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>21.42</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>1120</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <f aca="false">0.9*B7</f>
         <v>1008</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>4.45</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="2" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>1244</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <f aca="false">0.9*B8</f>
         <v>1119.6</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>3.61</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>2673</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <f aca="false">0.9*B9</f>
         <v>2405.7</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>3.71</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>48</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="3" t="n">
+      <c r="B10" s="4" t="n">
         <v>554</v>
       </c>
-      <c r="C10" s="4" t="n">
+      <c r="C10" s="1" t="n">
         <f aca="false">0.9*B10</f>
         <v>498.6</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <v>2.34</v>
       </c>
-      <c r="E10" s="3" t="n">
+      <c r="E10" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>1440</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <f aca="false">0.9*B11</f>
         <v>1296</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <v>4.23</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>34.7</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E12" s="1"/>
+      <c r="E12" s="2"/>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>